<commit_message>
Evaluations: #21, Updated some erroneous selector characterizations.
</commit_message>
<xml_diff>
--- a/eval/e21/selector_text.xlsx
+++ b/eval/e21/selector_text.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6400" yWindow="0" windowWidth="28160" windowHeight="25080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1410,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1479,7 +1479,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1731,7 +1731,7 @@
         <v>3</v>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1759,7 +1759,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1983,7 +1983,7 @@
         <v>3</v>
       </c>
       <c r="D40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2011,7 +2011,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4">

</xml_diff>